<commit_message>
no data checks + post code parser
</commit_message>
<xml_diff>
--- a/data_entry_template.xlsx
+++ b/data_entry_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\TNT_forms_autofill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B268D77-4433-4B57-9EDB-30C442AB01F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B5D9D1-F2E1-4BC8-8488-2B599C287B3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="1650" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>